<commit_message>
Nouveau script + journal de bord
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_bord_Festivel.xlsx
+++ b/Documentation/Journal_de_bord_Festivel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke.CORNAZ\Documents\GitHub\Festivel\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Validation du MCD et du MLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clôture du Sprint 1 </t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Liasion à la base de donnée</t>
   </si>
 </sst>
 </file>
@@ -380,56 +389,56 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -715,7 +724,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,15 +740,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="1"/>
@@ -769,295 +778,307 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>44312</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>44319</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>44326</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="10">
+        <v>44326</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="20"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="21"/>
+      <c r="A7" s="10">
+        <v>44334</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="20"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="21"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="21"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="21"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="21"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="21"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="21"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="21"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="21"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="21"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="21"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="21"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="21"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="6"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="6"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="21"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="6"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="22"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="21"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="6"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F24" s="1"/>

</xml_diff>